<commit_message>
Add transit line selection with vehicle allocation in config file
- New filter strategy based on transit line id.
- Allocation of vehicle type based on transit line id.
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86D825F-BC53-488E-A44C-C1A150108DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BFC70C-BB3A-4708-B0FB-FC8D8ED59152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="12710" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="2" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
     <sheet name="vehicle_types" sheetId="5" r:id="rId2"/>
-    <sheet name="shunting_locations_on_route" sheetId="2" r:id="rId3"/>
-    <sheet name="depot_locations" sheetId="1" r:id="rId4"/>
-    <sheet name="maintenance_slots" sheetId="3" r:id="rId5"/>
+    <sheet name="transit_lines" sheetId="6" r:id="rId3"/>
+    <sheet name="shunting_locations_on_route" sheetId="2" r:id="rId4"/>
+    <sheet name="depot_locations" sheetId="1" r:id="rId5"/>
+    <sheet name="maintenance_slots" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$25</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="104">
   <si>
     <t>location_id</t>
   </si>
@@ -346,6 +347,15 @@
   </si>
   <si>
     <t>The coordinate reference system of the network</t>
+  </si>
+  <si>
+    <t>transit_line_id</t>
+  </si>
+  <si>
+    <t>vehicle_type</t>
+  </si>
+  <si>
+    <t>Note: This sheet is optional; if list is empty, no filter is applied.</t>
   </si>
 </sst>
 </file>
@@ -747,21 +757,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.81640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="129.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.15234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.84375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="6.4609375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="129.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -778,7 +788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -793,7 +803,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -807,7 +817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -821,7 +831,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -835,7 +845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -849,7 +859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -866,7 +876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -884,7 +894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -898,7 +908,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -915,7 +925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -932,7 +942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -950,7 +960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -967,7 +977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -981,7 +991,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -998,7 +1008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1015,7 +1025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1032,7 +1042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1050,7 +1060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1068,7 +1078,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1086,7 +1096,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1113,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1120,7 +1130,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1137,7 +1147,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1187,18 +1197,18 @@
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.23046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -1218,7 +1228,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1235,7 +1245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1258,6 +1268,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E31C2-14D1-4EB0-9548-0D6A0EA80330}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.3828125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455315F6-EE05-465E-98C9-4563FB409249}">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -1266,52 +1305,52 @@
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1321,7 +1360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319C589F-C9B8-4390-8C65-9522706FCF68}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1330,14 +1369,14 @@
       <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1390,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1362,7 +1401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1373,7 +1412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1384,7 +1423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1395,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1406,7 +1445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1417,7 +1456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1428,7 +1467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -1439,7 +1478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1450,7 +1489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -1461,7 +1500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1472,7 +1511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -1488,7 +1527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01B7B07-7F3C-4799-BD75-429B5670A61E}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -1497,14 +1536,14 @@
       <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1518,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1532,7 +1571,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -1546,7 +1585,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -1560,7 +1599,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -1574,7 +1613,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1588,7 +1627,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1602,7 +1641,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1616,7 +1655,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1630,7 +1669,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1644,7 +1683,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1658,7 +1697,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -1672,7 +1711,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -1686,7 +1725,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -1700,7 +1739,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -1714,7 +1753,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -1728,7 +1767,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>87</v>
       </c>

</xml_diff>